<commit_message>
fix(fixes_2): fix gantt and posts edit delete
</commit_message>
<xml_diff>
--- a/public/assets/files/DemoProject.xlsx
+++ b/public/assets/files/DemoProject.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t xml:space="preserve">End time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completed percentage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duration</t>
   </si>
   <si>
     <t xml:space="preserve">Project #1</t>
@@ -137,7 +131,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -154,8 +148,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -163,11 +161,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="11" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -250,10 +248,10 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39"/>
@@ -276,152 +274,136 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="5" t="n">
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="6" t="n">
         <v>43192</v>
       </c>
-      <c r="D2" s="5" t="n">
+      <c r="D2" s="6" t="n">
         <v>43192</v>
-      </c>
-      <c r="E2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="0" t="n">
-        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="6" t="n">
         <v>43192</v>
       </c>
-      <c r="D3" s="5" t="n">
+      <c r="D3" s="6" t="n">
         <v>43192</v>
       </c>
-      <c r="E3" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>17</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="7"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="7"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="7"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="7"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="6"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="7"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="7"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="6"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="7"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="6"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="7"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="7"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="7"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>